<commit_message>
Magnetic design calculations are added
</commit_message>
<xml_diff>
--- a/simulation report/Magnetic Design calculator.xlsx
+++ b/simulation report/Magnetic Design calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\EE464-PeakyConverters\simulation report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA37C3C-4A52-4B53-8598-1ECD664DE0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC1B5B5-1BB7-45D5-833F-85D712201091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>55928A2</t>
   </si>
@@ -154,13 +154,37 @@
   </si>
   <si>
     <t>Calculations are made with litz wire diameter of 4mm^2</t>
+  </si>
+  <si>
+    <t>00K4022E090</t>
+  </si>
+  <si>
+    <t>00K3515E090</t>
+  </si>
+  <si>
+    <t>00K6527E060</t>
+  </si>
+  <si>
+    <t>00K7228E060</t>
+  </si>
+  <si>
+    <t>0P45530EC</t>
+  </si>
+  <si>
+    <t>0P43517EC</t>
+  </si>
+  <si>
+    <t>0P45959EC</t>
+  </si>
+  <si>
+    <t>FX2238</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +225,15 @@
       <charset val="162"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -270,7 +307,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -291,6 +328,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,7 +799,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="8">
@@ -953,7 +1002,49 @@
         <v>30</v>
       </c>
     </row>
+    <row r="17" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Component list and designs on driver, controller added
</commit_message>
<xml_diff>
--- a/simulation report/Magnetic Design calculator.xlsx
+++ b/simulation report/Magnetic Design calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\EE464-PeakyConverters\simulation report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC1B5B5-1BB7-45D5-833F-85D712201091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BAD7BE-7273-4F33-A482-C2E2C97A8C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>55928A2</t>
   </si>
@@ -177,14 +177,46 @@
     <t>0P45959EC</t>
   </si>
   <si>
-    <t>FX2238</t>
+    <r>
+      <t xml:space="preserve">if turns ratio </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="162"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1:2</t>
+    </r>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>84.3</t>
+  </si>
+  <si>
+    <t>low AL</t>
+  </si>
+  <si>
+    <t>N1</t>
+  </si>
+  <si>
+    <t>N2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +264,14 @@
       <family val="2"/>
       <charset val="162"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,6 +299,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -331,15 +381,24 @@
     <xf numFmtId="49" fontId="2" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,7 +682,7 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1002,46 +1061,159 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="14" t="s">
+      <c r="B18" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="19" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="B19" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="19" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
+      <c r="B20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="19" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
+      <c r="B21" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+    </row>
+    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="15" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="B22" s="14">
+        <v>375</v>
+      </c>
+      <c r="C22" s="14">
+        <v>420</v>
+      </c>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14">
+        <v>4</v>
+      </c>
+      <c r="F22" s="14">
+        <v>8</v>
+      </c>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="16" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24" s="14">
+        <v>509</v>
+      </c>
+      <c r="C24" s="14">
+        <v>368</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14">
+        <v>5</v>
+      </c>
+      <c r="F24" s="14">
+        <v>10</v>
+      </c>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>